<commit_message>
added new round data and Tee Fairway column
</commit_message>
<xml_diff>
--- a/adams_golf_data/scorecards.xlsx
+++ b/adams_golf_data/scorecards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamlynch/Documents/HobbyWork/golf-tracker/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamlynch/Documents/HobbyWork/golf-tracker/adams_golf_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE9EFBB-B844-C042-86DE-186F6727F92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB26D4B-5950-D14E-859D-EB1A4F409FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{756941FC-0F4E-6742-AA79-FAEAEC5B4D2A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17400" activeTab="5" xr2:uid="{756941FC-0F4E-6742-AA79-FAEAEC5B4D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rounds" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CGC-W-05232025" sheetId="6" r:id="rId3"/>
     <sheet name="CGC-W-05302025" sheetId="7" r:id="rId4"/>
     <sheet name="CGC-W-05312025" sheetId="8" r:id="rId5"/>
+    <sheet name="CGC-W-06022025" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="17">
   <si>
     <t>Course Code</t>
   </si>
@@ -79,13 +80,25 @@
   </si>
   <si>
     <t>Round Code</t>
+  </si>
+  <si>
+    <t>CGC-W-06022025</t>
+  </si>
+  <si>
+    <t>Tee Fairway</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +108,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036FC3A8-D8A6-2D4D-A81B-5BF9C0BDADE9}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,6 +546,17 @@
         <v>45808</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45810</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -533,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95E0240-19A8-DE46-8A81-C9A5EE553A21}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +576,7 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -552,16 +584,19 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -569,7 +604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -577,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -585,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -593,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -601,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -609,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -617,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -625,7 +660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -640,10 +675,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09ECA1A8-976A-7B4F-A8DF-CA5E7B9DA3B5}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,119 +686,122 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
@@ -774,10 +812,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863890F1-D659-3443-979B-25E69BFFFD58}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,119 +823,122 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>2</v>
       </c>
     </row>
@@ -908,10 +949,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DCB683-BB62-E044-A78D-C6E7B89BA21C}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,119 +960,337 @@
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BBC145-9685-CC40-A23A-74BB852F33D3}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
       <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
better dtype handing and test case
</commit_message>
<xml_diff>
--- a/adams_golf_data/scorecards.xlsx
+++ b/adams_golf_data/scorecards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamlynch/Documents/HobbyWork/golf-tracker/adams_golf_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB26D4B-5950-D14E-859D-EB1A4F409FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A66F336-AE1A-D445-A3D9-4185140ECD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17400" activeTab="5" xr2:uid="{756941FC-0F4E-6742-AA79-FAEAEC5B4D2A}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="29400" windowHeight="17400" activeTab="5" xr2:uid="{756941FC-0F4E-6742-AA79-FAEAEC5B4D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Rounds" sheetId="2" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,7 +815,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>